<commit_message>
Created Historgram of the full data join.  Added pictures that I inserted into the Google Doc.
</commit_message>
<xml_diff>
--- a/string-matching_tests/String_Matching_Histograms.xlsx
+++ b/string-matching_tests/String_Matching_Histograms.xlsx
@@ -4,15 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="24915" windowHeight="12330" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="24915" windowHeight="12330" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Histograms" sheetId="2" r:id="rId1"/>
     <sheet name="Pair Data" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="1B Run - Small Bin Size" sheetId="3" r:id="rId3"/>
+    <sheet name="1B Run - Larger Bin Size" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="histogram_numbers" localSheetId="3">'1B Run - Larger Bin Size'!$A$1:$C$22</definedName>
     <definedName name="output" localSheetId="1">'Pair Data'!$A$2:$E$101</definedName>
+    <definedName name="results" localSheetId="2">'1B Run - Small Bin Size'!$A$1:$C$101</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -20,8 +23,26 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="output" type="6" refreshedVersion="3" background="1" saveData="1">
+  <connection id="1" name="histogram_numbers" type="6" refreshedVersion="3" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\olyhaa\Documents\My Dropbox\histogram_numbers.dat" space="1" consecutive="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="output" type="6" refreshedVersion="3" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Amanda\Coursework\CSCI-4960\Assignments\Final_Project\String_Testing\output.ttl" tab="0" comma="1">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="results" type="6" refreshedVersion="3" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\olyhaa\Documents\My Dropbox\results.dat" space="1" consecutive="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -33,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
   <si>
     <t>Length 1</t>
   </si>
@@ -181,6 +202,33 @@
   <si>
     <t>Correct Set</t>
   </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>Above 0.65</t>
+  </si>
+  <si>
+    <t>Below 0.65</t>
+  </si>
+  <si>
+    <t>Above 0.7</t>
+  </si>
+  <si>
+    <t>Below 0.7</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
 </sst>
 </file>
 
@@ -477,11 +525,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="53577984"/>
-        <c:axId val="53584640"/>
+        <c:axId val="50334336"/>
+        <c:axId val="50340992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="53577984"/>
+        <c:axId val="50334336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -506,14 +554,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53584640"/>
+        <c:crossAx val="50340992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53584640"/>
+        <c:axId val="50340992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -539,7 +587,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53577984"/>
+        <c:crossAx val="50334336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -552,7 +600,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -777,11 +825,11 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="35"/>
-        <c:axId val="53605888"/>
-        <c:axId val="53607808"/>
+        <c:axId val="50362240"/>
+        <c:axId val="50384896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="53605888"/>
+        <c:axId val="50362240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -806,14 +854,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53607808"/>
+        <c:crossAx val="50384896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53607808"/>
+        <c:axId val="50384896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -839,7 +887,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53605888"/>
+        <c:crossAx val="50362240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -852,7 +900,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1604,11 +1652,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="55878784"/>
-        <c:axId val="55880704"/>
+        <c:axId val="63702528"/>
+        <c:axId val="63704448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="55878784"/>
+        <c:axId val="63702528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1634,12 +1682,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55880704"/>
+        <c:crossAx val="63704448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="55880704"/>
+        <c:axId val="63704448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1665,7 +1713,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55878784"/>
+        <c:crossAx val="63702528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1678,7 +1726,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1709,7 +1757,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout>
@@ -1717,10 +1764,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.3829776200881135E-2"/>
+          <c:x val="9.382977620088119E-2"/>
           <c:y val="0.10145282472602317"/>
           <c:w val="0.70637356677348595"/>
-          <c:h val="0.76910557066442686"/>
+          <c:h val="0.76910557066442753"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2445,11 +2492,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="55922688"/>
-        <c:axId val="55924608"/>
+        <c:axId val="63742336"/>
+        <c:axId val="63744256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="55922688"/>
+        <c:axId val="63742336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2471,16 +2518,15 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55924608"/>
+        <c:crossAx val="63744256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="55924608"/>
+        <c:axId val="63744256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2502,24 +2548,1015 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55922688"/>
+        <c:crossAx val="63742336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Similarity Measurements - Histogram</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> - Full Set</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.6463962583097581E-2"/>
+          <c:y val="1.6986836527725965E-2"/>
+          <c:w val="0.92353603741690238"/>
+          <c:h val="0.87868226755922352"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'1B Run - Small Bin Size'!$A$2:$A$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0000000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.9999999999999992E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.10999999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.11999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.12999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.13999999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.18000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.19000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.20000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.21000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.22000000000000006</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.23000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.24000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.25000000000000006</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.26000000000000006</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.27000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.28000000000000008</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.29000000000000009</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.3000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.31000000000000011</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.32000000000000012</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.33000000000000013</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.34000000000000014</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.35000000000000014</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.36000000000000015</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.37000000000000016</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.38000000000000017</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.39000000000000018</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.40000000000000019</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.4100000000000002</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.42000000000000021</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.43000000000000022</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.44000000000000022</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.45000000000000023</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.46000000000000024</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.47000000000000025</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.48000000000000026</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.49000000000000027</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.50000000000000022</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.51000000000000023</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.52000000000000024</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.53000000000000025</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.54000000000000026</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.55000000000000027</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.56000000000000028</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.57000000000000028</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.58000000000000029</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.5900000000000003</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.60000000000000031</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.61000000000000032</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.62000000000000033</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.63000000000000034</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.64000000000000035</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.65000000000000036</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.66000000000000036</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.67000000000000037</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.68000000000000038</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.69000000000000039</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.7000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.71000000000000041</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.72000000000000042</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.73000000000000043</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.74000000000000044</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.75000000000000044</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.76000000000000045</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.77000000000000046</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.78000000000000047</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.79000000000000048</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.80000000000000049</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.8100000000000005</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.82000000000000051</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.83000000000000052</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.84000000000000052</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.85000000000000053</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.86000000000000054</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.87000000000000055</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.88000000000000056</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.89000000000000057</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.90000000000000058</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.91000000000000059</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.9200000000000006</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.9300000000000006</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.94000000000000061</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.95000000000000062</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.96000000000000063</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.97000000000000064</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.98000000000000065</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.99000000000000066</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'1B Run - Small Bin Size'!$B$2:$B$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>279</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>293</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>388</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>505</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>441</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>535</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>882</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>685</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1313</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2415</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>276</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2336</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2155</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2907</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4406</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5434</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>7682</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>11801</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>14726</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>26783</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>23624</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>42901</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>56114</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>82649</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>117519</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>205759</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>287085</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>403027</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>726336</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1298599</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1599423</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>3063273</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>4391405</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>7210044</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>12998202</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>11945308</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>19332562</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>24388287</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>32445015</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>28262410</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>44911514</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>38710726</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>35138796</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>31604539</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>27437647</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>21579356</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>19308622</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>16395630</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>13204728</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>9669512</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>10049240</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>6732083</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>5748622</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>4510013</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>3279435</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1935693</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1019812</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>684442</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>214395</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>634899</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="63761792"/>
+        <c:axId val="102188160"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="63761792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1100" b="1" i="0" baseline="0"/>
+                  <a:t>Degree of Similarity (range of 0.01)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1100"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="102188160"/>
+        <c:crosses val="autoZero"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="10"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="102188160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Count</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="63761792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Similarity Measurements</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> - Histogram - Full Set</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'1B Run - Larger Bin Size'!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'1B Run - Larger Bin Size'!$B$2:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>291</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>639</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1906</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3621</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14289</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>54514</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>334719</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2606070</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>23384717</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>122565948</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>175132139</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>82828931</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>30063990</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4744644</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="102107776"/>
+        <c:axId val="111394816"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="102107776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Degree of Similarity (range of 0.05)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="111394816"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="111394816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Count</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="102107776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2655,8 +3692,86 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>521804</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>91109</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>256760</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>8283</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>304799</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85723</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="output" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="output" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="results" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="histogram_numbers" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2946,8 +4061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BI102"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="BG33" sqref="BG33"/>
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BH31" sqref="BH31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14748,7 +15863,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AE41" sqref="AE41"/>
     </sheetView>
   </sheetViews>
@@ -16797,12 +17912,1188 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1">
+        <v>441736711</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <f>A2+0.01</f>
+        <v>0.01</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <f t="shared" ref="A4:A67" si="0">A3+0.01</f>
+        <v>0.02</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4">
+        <f>SUM(B67:B101)</f>
+        <v>441326439</v>
+      </c>
+      <c r="G4">
+        <f>F4/C1*100</f>
+        <v>99.907122955873135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>0.03</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5">
+        <f>SUM(B2:B66)</f>
+        <v>410272</v>
+      </c>
+      <c r="G5">
+        <f>F5/C1*100</f>
+        <v>9.2877044126857738E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>0.05</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7">
+        <f>SUM(B72:B101)</f>
+        <v>438405633</v>
+      </c>
+      <c r="G7">
+        <f>F7/C1*100</f>
+        <v>99.24591325170617</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>6.0000000000000005E-2</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8">
+        <f>SUM(B2:B71)</f>
+        <v>3331078</v>
+      </c>
+      <c r="G8">
+        <f>F8/C1*100</f>
+        <v>0.75408674829382694</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>0.08</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>0.09</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>0.10999999999999999</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>0.11999999999999998</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>0.12999999999999998</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>0.16</v>
+      </c>
+      <c r="B18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>0.17</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>0.18000000000000002</v>
+      </c>
+      <c r="B20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>0.19000000000000003</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>0.20000000000000004</v>
+      </c>
+      <c r="B22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>0.21000000000000005</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>0.22000000000000006</v>
+      </c>
+      <c r="B24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>0.23000000000000007</v>
+      </c>
+      <c r="B25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>0.24000000000000007</v>
+      </c>
+      <c r="B26">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>0.25000000000000006</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>0.26000000000000006</v>
+      </c>
+      <c r="B28">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>0.27000000000000007</v>
+      </c>
+      <c r="B29">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>0.28000000000000008</v>
+      </c>
+      <c r="B30">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>0.29000000000000009</v>
+      </c>
+      <c r="B31">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>0.3000000000000001</v>
+      </c>
+      <c r="B32">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>0.31000000000000011</v>
+      </c>
+      <c r="B33">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>0.32000000000000012</v>
+      </c>
+      <c r="B34">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>0.33000000000000013</v>
+      </c>
+      <c r="B35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>0.34000000000000014</v>
+      </c>
+      <c r="B36">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>0.35000000000000014</v>
+      </c>
+      <c r="B37">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>0.36000000000000015</v>
+      </c>
+      <c r="B38">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>0.37000000000000016</v>
+      </c>
+      <c r="B39">
+        <v>147</v>
+      </c>
+      <c r="G39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>0.38000000000000017</v>
+      </c>
+      <c r="B40">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>0.39000000000000018</v>
+      </c>
+      <c r="B41">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>0.40000000000000019</v>
+      </c>
+      <c r="B42">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43">
+        <f t="shared" si="0"/>
+        <v>0.4100000000000002</v>
+      </c>
+      <c r="B43">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44">
+        <f t="shared" si="0"/>
+        <v>0.42000000000000021</v>
+      </c>
+      <c r="B44">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45">
+        <f t="shared" si="0"/>
+        <v>0.43000000000000022</v>
+      </c>
+      <c r="B45">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46">
+        <f t="shared" si="0"/>
+        <v>0.44000000000000022</v>
+      </c>
+      <c r="B46">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47">
+        <f t="shared" si="0"/>
+        <v>0.45000000000000023</v>
+      </c>
+      <c r="B47">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48">
+        <f t="shared" si="0"/>
+        <v>0.46000000000000024</v>
+      </c>
+      <c r="B48">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49">
+        <f t="shared" si="0"/>
+        <v>0.47000000000000025</v>
+      </c>
+      <c r="B49">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50">
+        <f t="shared" si="0"/>
+        <v>0.48000000000000026</v>
+      </c>
+      <c r="B50">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51">
+        <f t="shared" si="0"/>
+        <v>0.49000000000000027</v>
+      </c>
+      <c r="B51">
+        <v>2415</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52">
+        <f t="shared" si="0"/>
+        <v>0.50000000000000022</v>
+      </c>
+      <c r="B52">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53">
+        <f t="shared" si="0"/>
+        <v>0.51000000000000023</v>
+      </c>
+      <c r="B53">
+        <v>2336</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54">
+        <f t="shared" si="0"/>
+        <v>0.52000000000000024</v>
+      </c>
+      <c r="B54">
+        <v>2155</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55">
+        <f t="shared" si="0"/>
+        <v>0.53000000000000025</v>
+      </c>
+      <c r="B55">
+        <v>2907</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56">
+        <f t="shared" si="0"/>
+        <v>0.54000000000000026</v>
+      </c>
+      <c r="B56">
+        <v>4406</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57">
+        <f t="shared" si="0"/>
+        <v>0.55000000000000027</v>
+      </c>
+      <c r="B57">
+        <v>5434</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58">
+        <f t="shared" si="0"/>
+        <v>0.56000000000000028</v>
+      </c>
+      <c r="B58">
+        <v>7682</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59">
+        <f t="shared" si="0"/>
+        <v>0.57000000000000028</v>
+      </c>
+      <c r="B59">
+        <v>11801</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60">
+        <f t="shared" si="0"/>
+        <v>0.58000000000000029</v>
+      </c>
+      <c r="B60">
+        <v>14726</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61">
+        <f t="shared" si="0"/>
+        <v>0.5900000000000003</v>
+      </c>
+      <c r="B61">
+        <v>26783</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62">
+        <f t="shared" si="0"/>
+        <v>0.60000000000000031</v>
+      </c>
+      <c r="B62">
+        <v>23624</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63">
+        <f t="shared" si="0"/>
+        <v>0.61000000000000032</v>
+      </c>
+      <c r="B63">
+        <v>42901</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64">
+        <f t="shared" si="0"/>
+        <v>0.62000000000000033</v>
+      </c>
+      <c r="B64">
+        <v>56114</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65">
+        <f t="shared" si="0"/>
+        <v>0.63000000000000034</v>
+      </c>
+      <c r="B65">
+        <v>82649</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66">
+        <f t="shared" si="0"/>
+        <v>0.64000000000000035</v>
+      </c>
+      <c r="B66">
+        <v>117519</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67">
+        <f t="shared" si="0"/>
+        <v>0.65000000000000036</v>
+      </c>
+      <c r="B67">
+        <v>205759</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68">
+        <f t="shared" ref="A68:A101" si="1">A67+0.01</f>
+        <v>0.66000000000000036</v>
+      </c>
+      <c r="B68">
+        <v>287085</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69">
+        <f t="shared" si="1"/>
+        <v>0.67000000000000037</v>
+      </c>
+      <c r="B69">
+        <v>403027</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70">
+        <f t="shared" si="1"/>
+        <v>0.68000000000000038</v>
+      </c>
+      <c r="B70">
+        <v>726336</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71">
+        <f t="shared" si="1"/>
+        <v>0.69000000000000039</v>
+      </c>
+      <c r="B71">
+        <v>1298599</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72">
+        <f t="shared" si="1"/>
+        <v>0.7000000000000004</v>
+      </c>
+      <c r="B72">
+        <v>1599423</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73">
+        <f t="shared" si="1"/>
+        <v>0.71000000000000041</v>
+      </c>
+      <c r="B73">
+        <v>3063273</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74">
+        <f t="shared" si="1"/>
+        <v>0.72000000000000042</v>
+      </c>
+      <c r="B74">
+        <v>4391405</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75">
+        <f t="shared" si="1"/>
+        <v>0.73000000000000043</v>
+      </c>
+      <c r="B75">
+        <v>7210044</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76">
+        <f t="shared" si="1"/>
+        <v>0.74000000000000044</v>
+      </c>
+      <c r="B76">
+        <v>12998202</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77">
+        <f t="shared" si="1"/>
+        <v>0.75000000000000044</v>
+      </c>
+      <c r="B77">
+        <v>11945308</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78">
+        <f t="shared" si="1"/>
+        <v>0.76000000000000045</v>
+      </c>
+      <c r="B78">
+        <v>19332562</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79">
+        <f t="shared" si="1"/>
+        <v>0.77000000000000046</v>
+      </c>
+      <c r="B79">
+        <v>24388287</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80">
+        <f t="shared" si="1"/>
+        <v>0.78000000000000047</v>
+      </c>
+      <c r="B80">
+        <v>32445015</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81">
+        <f t="shared" si="1"/>
+        <v>0.79000000000000048</v>
+      </c>
+      <c r="B81">
+        <v>28262410</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82">
+        <f t="shared" si="1"/>
+        <v>0.80000000000000049</v>
+      </c>
+      <c r="B82">
+        <v>44911514</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83">
+        <f t="shared" si="1"/>
+        <v>0.8100000000000005</v>
+      </c>
+      <c r="B83">
+        <v>38710726</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84">
+        <f t="shared" si="1"/>
+        <v>0.82000000000000051</v>
+      </c>
+      <c r="B84">
+        <v>35138796</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85">
+        <f t="shared" si="1"/>
+        <v>0.83000000000000052</v>
+      </c>
+      <c r="B85">
+        <v>31604539</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86">
+        <f t="shared" si="1"/>
+        <v>0.84000000000000052</v>
+      </c>
+      <c r="B86">
+        <v>27437647</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87">
+        <f t="shared" si="1"/>
+        <v>0.85000000000000053</v>
+      </c>
+      <c r="B87">
+        <v>21579356</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88">
+        <f t="shared" si="1"/>
+        <v>0.86000000000000054</v>
+      </c>
+      <c r="B88">
+        <v>19308622</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89">
+        <f t="shared" si="1"/>
+        <v>0.87000000000000055</v>
+      </c>
+      <c r="B89">
+        <v>16395630</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90">
+        <f t="shared" si="1"/>
+        <v>0.88000000000000056</v>
+      </c>
+      <c r="B90">
+        <v>13204728</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91">
+        <f t="shared" si="1"/>
+        <v>0.89000000000000057</v>
+      </c>
+      <c r="B91">
+        <v>9669512</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92">
+        <f t="shared" si="1"/>
+        <v>0.90000000000000058</v>
+      </c>
+      <c r="B92">
+        <v>10049240</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93">
+        <f t="shared" si="1"/>
+        <v>0.91000000000000059</v>
+      </c>
+      <c r="B93">
+        <v>6732083</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94">
+        <f t="shared" si="1"/>
+        <v>0.9200000000000006</v>
+      </c>
+      <c r="B94">
+        <v>5748622</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95">
+        <f t="shared" si="1"/>
+        <v>0.9300000000000006</v>
+      </c>
+      <c r="B95">
+        <v>4510013</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96">
+        <f t="shared" si="1"/>
+        <v>0.94000000000000061</v>
+      </c>
+      <c r="B96">
+        <v>3279435</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97">
+        <f t="shared" si="1"/>
+        <v>0.95000000000000062</v>
+      </c>
+      <c r="B97">
+        <v>1935693</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98">
+        <f t="shared" si="1"/>
+        <v>0.96000000000000063</v>
+      </c>
+      <c r="B98">
+        <v>1019812</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99">
+        <f t="shared" si="1"/>
+        <v>0.97000000000000064</v>
+      </c>
+      <c r="B99">
+        <v>684442</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100">
+        <f t="shared" si="1"/>
+        <v>0.98000000000000065</v>
+      </c>
+      <c r="B100">
+        <v>214395</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101">
+        <f t="shared" si="1"/>
+        <v>0.99000000000000066</v>
+      </c>
+      <c r="B101">
+        <v>634899</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1">
+        <v>441736711</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>0.05</v>
+      </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>0.1</v>
+      </c>
+      <c r="B4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>0.15</v>
+      </c>
+      <c r="B5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>0.2</v>
+      </c>
+      <c r="B6">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>0.25</v>
+      </c>
+      <c r="B7">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>0.3</v>
+      </c>
+      <c r="B8">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>0.35</v>
+      </c>
+      <c r="B9">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>0.4</v>
+      </c>
+      <c r="B10">
+        <v>1906</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>0.45</v>
+      </c>
+      <c r="B11">
+        <v>3621</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>0.5</v>
+      </c>
+      <c r="B12">
+        <v>14289</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B13">
+        <v>54514</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>0.6</v>
+      </c>
+      <c r="B14">
+        <v>334719</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>0.65</v>
+      </c>
+      <c r="B15">
+        <v>2606070</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>0.7</v>
+      </c>
+      <c r="B16">
+        <v>23384717</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>0.75</v>
+      </c>
+      <c r="B17">
+        <v>122565948</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>0.8</v>
+      </c>
+      <c r="B18">
+        <v>175132139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>0.85</v>
+      </c>
+      <c r="B19">
+        <v>82828931</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>0.9</v>
+      </c>
+      <c r="B20">
+        <v>30063990</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>0.95</v>
+      </c>
+      <c r="B21">
+        <v>4744644</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22">
+        <v>0.82113199999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>